<commit_message>
arreglo del modelo y django
</commit_message>
<xml_diff>
--- a/PRUEBAS.xlsx
+++ b/PRUEBAS.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julio\Desktop\PROYECTO IA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alienware\Desktop\PROYECTO-DE-INTELIGENICA-ARTIFICIAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CB9E732-430F-42EF-9C44-8B0832E6F39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9FA9DC-58F5-4F70-B597-A72750882DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10770" yWindow="3495" windowWidth="16545" windowHeight="11835" xr2:uid="{02B5377D-6E55-496F-8807-09BC0ED98745}"/>
+    <workbookView xWindow="4110" yWindow="4110" windowWidth="21600" windowHeight="11835" xr2:uid="{02B5377D-6E55-496F-8807-09BC0ED98745}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1 " sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,18 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>SPLIT</t>
+    <t>alpha</t>
   </si>
   <si>
-    <t>test_size=0.2, random_state=42</t>
-  </si>
-  <si>
-    <t>test_size=0.33, random_state=155</t>
-  </si>
-  <si>
-    <t>5 K-FOLDS</t>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -55,7 +49,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -65,18 +59,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -112,11 +100,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -138,23 +133,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>295276</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>247090</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>452717</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3186289</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1571626</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>739583</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1076487</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="2" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{601319A8-76FF-5F78-2F70-07AFB2FA47D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{627AE392-A06D-4EDC-BE9A-45B484B70EFC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -170,8 +165,184 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2762250" y="809626"/>
-          <a:ext cx="3167239" cy="1276350"/>
+          <a:off x="6208619" y="710452"/>
+          <a:ext cx="4593846" cy="3178711"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>812427</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>440952</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1207431</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1045116</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7565A4-A451-48C0-A0D5-F922F1D0E5F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10875309" y="698687"/>
+          <a:ext cx="4496357" cy="3159105"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2171942</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>790675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC58F8D0-17C6-40EB-9F7F-4479849C26EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3181350" y="333375"/>
+          <a:ext cx="1733792" cy="714475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2200521</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1105014</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D84EADD5-8834-41BF-9AE8-94E9003760FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3181350" y="1400175"/>
+          <a:ext cx="1762371" cy="819264"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2191007</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>952616</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD3B05AD-FD56-4C23-85CD-4B57FFFFB974}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3095625" y="2933700"/>
+          <a:ext cx="1838582" cy="828791"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -499,14 +670,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1E4E86-3461-4402-B987-7952CD01746E}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7495D35-665A-406C-81FD-07538FC7D433}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.07421875" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="26.07421875" bestFit="1" customWidth="1"/>
   </cols>
@@ -515,32 +686,37 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>0.78139999999999998</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+    <row r="2" spans="1:3" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>2.5</v>
       </c>
       <c r="B2" s="2">
-        <v>0.78200000000000003</v>
+        <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
+      <c r="A3" s="3">
+        <v>1</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.78210000000000002</v>
+      <c r="B3" s="4">
+        <v>5</v>
       </c>
       <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
prueba de mejora de modelo a 0.802
</commit_message>
<xml_diff>
--- a/PRUEBAS.xlsx
+++ b/PRUEBAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alienware\Desktop\PROYECTO-DE-INTELIGENICA-ARTIFICIAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9FA9DC-58F5-4F70-B597-A72750882DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2ABE5C6-1126-4203-AD07-7012ACFDC1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="4110" windowWidth="21600" windowHeight="11835" xr2:uid="{02B5377D-6E55-496F-8807-09BC0ED98745}"/>
+    <workbookView xWindow="6615" yWindow="3165" windowWidth="21600" windowHeight="11835" xr2:uid="{02B5377D-6E55-496F-8807-09BC0ED98745}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1 " sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -106,7 +106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -351,6 +351,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2171950</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>896026</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFCB8897-4760-FC20-49C3-69D2335A301A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3115235" y="4000500"/>
+          <a:ext cx="1790950" cy="828791"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -671,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7495D35-665A-406C-81FD-07538FC7D433}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.07421875" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -718,6 +762,15 @@
       </c>
       <c r="C4" s="1"/>
     </row>
+    <row r="5" spans="1:3" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>90</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>